<commit_message>
LH: Added 2 papers
</commit_message>
<xml_diff>
--- a/Cols_draft_M5.xlsx
+++ b/Cols_draft_M5.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lydia\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0749EE3-C6D7-4E2B-A6AF-8DA6F9F05482}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D58A43F-BDA7-4F90-AC29-947173718D2D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{36676770-CB25-F949-8228-BA136C80F5EB}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="72">
   <si>
     <t>Link to article</t>
   </si>
@@ -252,12 +252,78 @@
   <si>
     <t>Lydia Hodgins</t>
   </si>
+  <si>
+    <t>Ioan</t>
+  </si>
+  <si>
+    <t>Cancer Cell Membrane-Coated Nanoparticles for Anticancer Vaccination and Drug Delivery</t>
+  </si>
+  <si>
+    <t>https://pubs.acs.org/doi/full/10.1021/nl500618u</t>
+  </si>
+  <si>
+    <t>Ioan Duchastel</t>
+  </si>
+  <si>
+    <t>Qualitative study with a lot of details on the experimental procedure, to the reagents used in every steps to the tools used in the experiment. Not 5/5 as some of the tools used are expensive but not a big deal. Image analysis can be done on open source software so overall pretty thorough and good study to follow</t>
+  </si>
+  <si>
+    <t>Effective cancer targeting and imaging using macrophage membranecamouflaged upconversion nanoparticles</t>
+  </si>
+  <si>
+    <t>https://onlinelibrary.wiley.com/doi/abs/10.1002/jbm.a.35927</t>
+  </si>
+  <si>
+    <t>Qualitative study with a decent amount of detail, methods are just enough for this paper, you can still access them through other related papers (which seems to be to get more citations than anything) but reagent concentrations are severely lacking, making it quite difficult to reproduce.</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Single-molecule tracking reveals the functional allocation, </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>in vivo</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t> interactions, and spatial organization of universal transcription factor NusG</t>
+    </r>
+  </si>
+  <si>
+    <t>https://doi.org/10.1016/j.molcel.2024.01.025</t>
+  </si>
+  <si>
+    <t>I left evaluating quality of experimental desing until the end because I felt that the points I was going to make in it fit better in the next three categories. When I returned to it I mostly reiterated the points I had made previously. I am also not sure how we are deciding the values to put int the replicability and reproducibility category - is it an average of the blue columns or just a general observation?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Single molecule microscopy reveals key physical features of repair foci in living cells </t>
+  </si>
+  <si>
+    <t>https://doi.org/10.7554/eLife.60577</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="13">
+  <fonts count="15">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -350,6 +416,19 @@
       <sz val="12"/>
       <color theme="3" tint="0.499984740745262"/>
       <name val="Aptos Narrow"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="12"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -493,7 +572,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -581,6 +660,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -994,8 +1076,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{037553EA-793E-E147-BDF6-0B4A3FE59E4A}">
   <dimension ref="A1:M55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" zoomScale="94" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="F28" sqref="F28"/>
+    <sheetView tabSelected="1" topLeftCell="H14" zoomScale="94" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="M25" sqref="M25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
@@ -1661,39 +1743,81 @@
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
-      <c r="B24" s="6"/>
-      <c r="C24" s="6"/>
-      <c r="D24" s="6"/>
+      <c r="B24" s="34" t="s">
+        <v>67</v>
+      </c>
+      <c r="C24" s="6">
+        <v>2024</v>
+      </c>
+      <c r="D24" s="17" t="s">
+        <v>68</v>
+      </c>
       <c r="E24" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="F24" s="6"/>
-      <c r="G24" s="6"/>
-      <c r="H24" s="6"/>
-      <c r="I24" s="6"/>
-      <c r="J24" s="6"/>
-      <c r="K24" s="6"/>
-      <c r="L24" s="6"/>
-      <c r="M24" s="6"/>
+      <c r="F24" s="22">
+        <v>5</v>
+      </c>
+      <c r="G24" s="22">
+        <v>5</v>
+      </c>
+      <c r="H24" s="22">
+        <v>5</v>
+      </c>
+      <c r="I24" s="22">
+        <v>4</v>
+      </c>
+      <c r="J24" s="22">
+        <v>3</v>
+      </c>
+      <c r="K24" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="L24" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="M24" s="6" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row r="25" spans="1:13" s="1" customFormat="1" ht="22.95" customHeight="1">
       <c r="A25" s="2">
         <f t="shared" si="0"/>
         <v>21</v>
       </c>
-      <c r="B25" s="6"/>
-      <c r="C25" s="6"/>
-      <c r="D25" s="6"/>
+      <c r="B25" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="C25" s="6">
+        <v>2021</v>
+      </c>
+      <c r="D25" s="17" t="s">
+        <v>71</v>
+      </c>
       <c r="E25" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="F25" s="6"/>
-      <c r="G25" s="6"/>
-      <c r="H25" s="6"/>
-      <c r="I25" s="6"/>
-      <c r="J25" s="6"/>
-      <c r="K25" s="6"/>
-      <c r="L25" s="6"/>
+      <c r="F25" s="6">
+        <v>5</v>
+      </c>
+      <c r="G25" s="6">
+        <v>4</v>
+      </c>
+      <c r="H25" s="6">
+        <v>4</v>
+      </c>
+      <c r="I25" s="6">
+        <v>5</v>
+      </c>
+      <c r="J25" s="6">
+        <v>1</v>
+      </c>
+      <c r="K25" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="L25" s="6" t="s">
+        <v>46</v>
+      </c>
       <c r="M25" s="6"/>
     </row>
     <row r="26" spans="1:13" s="1" customFormat="1">
@@ -1756,41 +1880,89 @@
       <c r="L28" s="6"/>
       <c r="M28" s="6"/>
     </row>
-    <row r="29" spans="1:13" s="1" customFormat="1">
+    <row r="29" spans="1:13" s="1" customFormat="1" ht="21.6" customHeight="1">
       <c r="A29" s="2">
         <f t="shared" si="0"/>
         <v>25</v>
       </c>
-      <c r="B29" s="6"/>
-      <c r="C29" s="6"/>
-      <c r="D29" s="6"/>
-      <c r="E29" s="6"/>
-      <c r="F29" s="6"/>
-      <c r="G29" s="6"/>
-      <c r="H29" s="6"/>
-      <c r="I29" s="6"/>
-      <c r="J29" s="6"/>
-      <c r="K29" s="6"/>
-      <c r="L29" s="6"/>
-      <c r="M29" s="6"/>
-    </row>
-    <row r="30" spans="1:13" s="1" customFormat="1">
+      <c r="B29" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="C29" s="6">
+        <v>2014</v>
+      </c>
+      <c r="D29" s="17" t="s">
+        <v>61</v>
+      </c>
+      <c r="E29" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="F29" s="6">
+        <v>2</v>
+      </c>
+      <c r="G29" s="6">
+        <v>5</v>
+      </c>
+      <c r="H29" s="6">
+        <v>5</v>
+      </c>
+      <c r="I29" s="6">
+        <v>4</v>
+      </c>
+      <c r="J29" s="6">
+        <v>4</v>
+      </c>
+      <c r="K29" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="L29" s="6">
+        <v>4</v>
+      </c>
+      <c r="M29" s="6" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" s="1" customFormat="1" ht="27" customHeight="1">
       <c r="A30" s="2">
         <f t="shared" si="0"/>
         <v>26</v>
       </c>
-      <c r="B30" s="6"/>
-      <c r="C30" s="6"/>
-      <c r="D30" s="6"/>
-      <c r="E30" s="6"/>
-      <c r="F30" s="6"/>
-      <c r="G30" s="6"/>
-      <c r="H30" s="6"/>
-      <c r="I30" s="6"/>
-      <c r="J30" s="6"/>
-      <c r="K30" s="6"/>
-      <c r="L30" s="6"/>
-      <c r="M30" s="6"/>
+      <c r="B30" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="C30" s="6">
+        <v>2016</v>
+      </c>
+      <c r="D30" s="17" t="s">
+        <v>65</v>
+      </c>
+      <c r="E30" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="F30" s="6">
+        <v>2</v>
+      </c>
+      <c r="G30" s="6">
+        <v>4</v>
+      </c>
+      <c r="H30" s="6">
+        <v>3</v>
+      </c>
+      <c r="I30" s="6">
+        <v>5</v>
+      </c>
+      <c r="J30" s="6">
+        <v>4</v>
+      </c>
+      <c r="K30" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="L30" s="6">
+        <v>4</v>
+      </c>
+      <c r="M30" s="6" t="s">
+        <v>66</v>
+      </c>
     </row>
     <row r="31" spans="1:13" s="1" customFormat="1" ht="21" customHeight="1">
       <c r="A31" s="2">
@@ -1800,7 +1972,9 @@
       <c r="B31" s="6"/>
       <c r="C31" s="6"/>
       <c r="D31" s="6"/>
-      <c r="E31" s="6"/>
+      <c r="E31" s="6" t="s">
+        <v>59</v>
+      </c>
       <c r="F31" s="6"/>
       <c r="G31" s="6"/>
       <c r="H31" s="6"/>
@@ -1818,7 +1992,9 @@
       <c r="B32" s="6"/>
       <c r="C32" s="6"/>
       <c r="D32" s="6"/>
-      <c r="E32" s="6"/>
+      <c r="E32" s="6" t="s">
+        <v>59</v>
+      </c>
       <c r="F32" s="6"/>
       <c r="G32" s="6"/>
       <c r="H32" s="6"/>
@@ -1836,7 +2012,9 @@
       <c r="B33" s="6"/>
       <c r="C33" s="6"/>
       <c r="D33" s="6"/>
-      <c r="E33" s="6"/>
+      <c r="E33" s="6" t="s">
+        <v>59</v>
+      </c>
       <c r="F33" s="6"/>
       <c r="G33" s="6"/>
       <c r="H33" s="6"/>
@@ -2244,6 +2422,10 @@
     <hyperlink ref="D11" r:id="rId4" xr:uid="{05674F12-7BCD-F047-B51E-2A47BBB4405F}"/>
     <hyperlink ref="D19" r:id="rId5" xr:uid="{800EF91D-8504-4040-BB43-40198693EDE2}"/>
     <hyperlink ref="D20" r:id="rId6" xr:uid="{95D8DD52-6892-0B41-BC31-4928BFD9FBFD}"/>
+    <hyperlink ref="D29" r:id="rId7" xr:uid="{08CA6207-3F6B-460E-92B7-F349FBEFB692}"/>
+    <hyperlink ref="D30" r:id="rId8" xr:uid="{65086669-9511-415C-A238-DD9BFFA9B52A}"/>
+    <hyperlink ref="D24" r:id="rId9" xr:uid="{1C69C3B3-F482-47A1-AE68-8270C3A61230}"/>
+    <hyperlink ref="D25" r:id="rId10" xr:uid="{B5ED07AE-40BD-47AC-A6EB-CCD4DF836BF1}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
LH: Adding my 2 papers
</commit_message>
<xml_diff>
--- a/Cols_draft_M5.xlsx
+++ b/Cols_draft_M5.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\QLSC600\Module 5\QLSC600D2_2025_M5A1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lydia\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8216108D-C699-4DD3-93E0-EBB43B05F6CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D58A43F-BDA7-4F90-AC29-947173718D2D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{36676770-CB25-F949-8228-BA136C80F5EB}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{36676770-CB25-F949-8228-BA136C80F5EB}"/>
   </bookViews>
   <sheets>
     <sheet name="Deadlines" sheetId="2" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="72">
   <si>
     <t>Link to article</t>
   </si>
@@ -276,12 +276,54 @@
   <si>
     <t>Qualitative study with a decent amount of detail, methods are just enough for this paper, you can still access them through other related papers (which seems to be to get more citations than anything) but reagent concentrations are severely lacking, making it quite difficult to reproduce.</t>
   </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Single-molecule tracking reveals the functional allocation, </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>in vivo</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t> interactions, and spatial organization of universal transcription factor NusG</t>
+    </r>
+  </si>
+  <si>
+    <t>https://doi.org/10.1016/j.molcel.2024.01.025</t>
+  </si>
+  <si>
+    <t>I left evaluating quality of experimental desing until the end because I felt that the points I was going to make in it fit better in the next three categories. When I returned to it I mostly reiterated the points I had made previously. I am also not sure how we are deciding the values to put int the replicability and reproducibility category - is it an average of the blue columns or just a general observation?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Single molecule microscopy reveals key physical features of repair foci in living cells </t>
+  </si>
+  <si>
+    <t>https://doi.org/10.7554/eLife.60577</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="13">
+  <fonts count="15">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -374,6 +416,19 @@
       <sz val="12"/>
       <color theme="3" tint="0.499984740745262"/>
       <name val="Aptos Narrow"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="12"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -517,7 +572,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -605,6 +660,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1018,8 +1076,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{037553EA-793E-E147-BDF6-0B4A3FE59E4A}">
   <dimension ref="A1:M55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" zoomScale="94" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="F31" sqref="F31"/>
+    <sheetView tabSelected="1" topLeftCell="H14" zoomScale="94" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="M25" sqref="M25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
@@ -1685,39 +1743,81 @@
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
-      <c r="B24" s="6"/>
-      <c r="C24" s="6"/>
-      <c r="D24" s="6"/>
+      <c r="B24" s="34" t="s">
+        <v>67</v>
+      </c>
+      <c r="C24" s="6">
+        <v>2024</v>
+      </c>
+      <c r="D24" s="17" t="s">
+        <v>68</v>
+      </c>
       <c r="E24" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="F24" s="6"/>
-      <c r="G24" s="6"/>
-      <c r="H24" s="6"/>
-      <c r="I24" s="6"/>
-      <c r="J24" s="6"/>
-      <c r="K24" s="6"/>
-      <c r="L24" s="6"/>
-      <c r="M24" s="6"/>
+      <c r="F24" s="22">
+        <v>5</v>
+      </c>
+      <c r="G24" s="22">
+        <v>5</v>
+      </c>
+      <c r="H24" s="22">
+        <v>5</v>
+      </c>
+      <c r="I24" s="22">
+        <v>4</v>
+      </c>
+      <c r="J24" s="22">
+        <v>3</v>
+      </c>
+      <c r="K24" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="L24" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="M24" s="6" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row r="25" spans="1:13" s="1" customFormat="1" ht="22.95" customHeight="1">
       <c r="A25" s="2">
         <f t="shared" si="0"/>
         <v>21</v>
       </c>
-      <c r="B25" s="6"/>
-      <c r="C25" s="6"/>
-      <c r="D25" s="6"/>
+      <c r="B25" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="C25" s="6">
+        <v>2021</v>
+      </c>
+      <c r="D25" s="17" t="s">
+        <v>71</v>
+      </c>
       <c r="E25" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="F25" s="6"/>
-      <c r="G25" s="6"/>
-      <c r="H25" s="6"/>
-      <c r="I25" s="6"/>
-      <c r="J25" s="6"/>
-      <c r="K25" s="6"/>
-      <c r="L25" s="6"/>
+      <c r="F25" s="6">
+        <v>5</v>
+      </c>
+      <c r="G25" s="6">
+        <v>4</v>
+      </c>
+      <c r="H25" s="6">
+        <v>4</v>
+      </c>
+      <c r="I25" s="6">
+        <v>5</v>
+      </c>
+      <c r="J25" s="6">
+        <v>1</v>
+      </c>
+      <c r="K25" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="L25" s="6" t="s">
+        <v>46</v>
+      </c>
       <c r="M25" s="6"/>
     </row>
     <row r="26" spans="1:13" s="1" customFormat="1">
@@ -2324,6 +2424,8 @@
     <hyperlink ref="D20" r:id="rId6" xr:uid="{95D8DD52-6892-0B41-BC31-4928BFD9FBFD}"/>
     <hyperlink ref="D29" r:id="rId7" xr:uid="{08CA6207-3F6B-460E-92B7-F349FBEFB692}"/>
     <hyperlink ref="D30" r:id="rId8" xr:uid="{65086669-9511-415C-A238-DD9BFFA9B52A}"/>
+    <hyperlink ref="D24" r:id="rId9" xr:uid="{1C69C3B3-F482-47A1-AE68-8270C3A61230}"/>
+    <hyperlink ref="D25" r:id="rId10" xr:uid="{B5ED07AE-40BD-47AC-A6EB-CCD4DF836BF1}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>